<commit_message>
[BI-1059] Updating files for name length
</commit_message>
<xml_diff>
--- a/src/test/resources/files/data_one_row.xlsx
+++ b/src/test/resources/files/data_one_row.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243-admin/IdeaProjects/bi-api/src/test/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24992BAC-80DD-BD49-BA43-7D0B2AA7C3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94F33DE-2E7D-364F-87D9-AFB5376333C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29440" windowHeight="15080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>Column</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Powdery Mildew Severity</t>
+  </si>
+  <si>
+    <t>PM_Leaf</t>
+  </si>
+  <si>
+    <t>Powdery Mildew severity, leaf</t>
   </si>
 </sst>
 </file>
@@ -819,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -902,7 +908,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>62</v>
@@ -929,7 +935,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>32</v>

</xml_diff>